<commit_message>
Endog.Retirement.Fixes:fugitive on gas.Fix to residential,iron&steel.
</commit_message>
<xml_diff>
--- a/EmissionFactors.xlsx
+++ b/EmissionFactors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38286175-CFF9-4704-87F3-614909C998DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9E6701-EB0D-44FE-ADC4-5F381D8618CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
+    <workbookView xWindow="1845" yWindow="135" windowWidth="26055" windowHeight="15600" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4788,6 +4790,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079636A6-22AB-49BE-AA94-1B152FC7212D}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7039,10 +7042,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA525E55-6D10-45A0-86EF-16765CC6C762}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="C1:AF478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="F471" sqref="F471"/>
+    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
+      <selection activeCell="D363" sqref="D363:G363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25483,21 +25487,17 @@
       <c r="C359" t="s">
         <v>712</v>
       </c>
-      <c r="D359">
-        <f>IF($P359&gt;0,0,IFERROR(INDEX(Factors!$C$5:$C$61,MATCH($J359,Factors!$B$5:$B$61,0)),0))</f>
-        <v>35.758799999999994</v>
-      </c>
-      <c r="E359">
-        <f>IF($P359&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J359,Factors!$B$5:$B$61,0)),0))</f>
-        <v>3.7799999999999997E-4</v>
-      </c>
-      <c r="F359">
-        <f>IF($P359&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J359,Factors!$B$5:$B$61,0)),0))</f>
-        <v>5.669999999999999E-4</v>
-      </c>
-      <c r="G359">
-        <f>IF(P359&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J359,Factors!$B$5:$B$61,0)),0))</f>
-        <v>35.942507999999997</v>
+      <c r="D359" s="8">
+        <v>0</v>
+      </c>
+      <c r="E359" s="8">
+        <v>0</v>
+      </c>
+      <c r="F359" s="8">
+        <v>0</v>
+      </c>
+      <c r="G359" s="8">
+        <v>0</v>
       </c>
       <c r="J359" t="str">
         <f t="shared" si="35"/>
@@ -25627,21 +25627,17 @@
       <c r="C362" t="s">
         <v>718</v>
       </c>
-      <c r="D362">
-        <f>IF($P362&gt;0,0,IFERROR(INDEX(Factors!$C$5:$C$61,MATCH($J362,Factors!$B$5:$B$61,0)),0))</f>
-        <v>96.25</v>
-      </c>
-      <c r="E362">
-        <f>IF($P362&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J362,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1E-3</v>
-      </c>
-      <c r="F362">
-        <f>IF($P362&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J362,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1.4E-3</v>
-      </c>
-      <c r="G362">
-        <f>IF(P362&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J362,Factors!$B$5:$B$61,0)),0))</f>
-        <v>96.704999999999998</v>
+      <c r="D362" s="8">
+        <v>0</v>
+      </c>
+      <c r="E362" s="8">
+        <v>0</v>
+      </c>
+      <c r="F362" s="8">
+        <v>0</v>
+      </c>
+      <c r="G362" s="8">
+        <v>0</v>
       </c>
       <c r="J362" t="str">
         <f t="shared" si="35"/>
@@ -31184,6 +31180,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD83B06F-7778-4674-BBAA-753F15EFCE57}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A6:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31231,6 +31228,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623B294C-93AD-4335-9A1B-23BCBE8C1678}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:W131"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fixes made to TCH_IND,TCH_PWR,P4C runs, CoalIPP prelim,forecast,DMD_PROJ
</commit_message>
<xml_diff>
--- a/EmissionFactors.xlsx
+++ b/EmissionFactors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6F36AF-592A-4539-8C01-EE1D281836C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305078AD-40A9-4026-92C4-ED6A500AAB8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2220" yWindow="-14985" windowWidth="24450" windowHeight="14295" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
+    <workbookView xWindow="1650" yWindow="195" windowWidth="25230" windowHeight="14940" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -44,6 +44,7 @@
     <author>tc={37E61244-2023-4973-BBB2-B89EBA2C85CA}</author>
     <author>tc={2A2805F6-FEBE-4A89-BE90-B22522BCA732}</author>
     <author>tc={6BC8B301-C25D-4243-8984-1D8083FBD633}</author>
+    <author>tc={F057E6D1-F0A4-43AE-A671-8DD980C81287}</author>
     <author>Fadiel Ahjum</author>
   </authors>
   <commentList>
@@ -71,7 +72,15 @@
     from Bryce, linked to amount of coke used for combustion.</t>
       </text>
     </comment>
-    <comment ref="C61" authorId="3" shapeId="0" xr:uid="{52625ABC-1A1C-441C-9203-49F352036B5C}">
+    <comment ref="E14" authorId="3" shapeId="0" xr:uid="{F057E6D1-F0A4-43AE-A671-8DD980C81287}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    adjusted to Match FBC coefficient - see TCH_PWR</t>
+      </text>
+    </comment>
+    <comment ref="C61" authorId="4" shapeId="0" xr:uid="{52625ABC-1A1C-441C-9203-49F352036B5C}">
       <text>
         <r>
           <rPr>
@@ -95,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F61" authorId="3" shapeId="0" xr:uid="{0CDECC13-11BC-4EA3-B18D-694980D9EA7E}">
+    <comment ref="F61" authorId="4" shapeId="0" xr:uid="{0CDECC13-11BC-4EA3-B18D-694980D9EA7E}">
       <text>
         <r>
           <rPr>
@@ -4286,7 +4295,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4347,6 +4356,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4434,7 +4449,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -4449,6 +4464,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -4472,6 +4488,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Bruno Merven" id="{B37ECF2F-7DD9-4573-B8C3-8678149F6950}" userId="Bruno Merven" providerId="None"/>
   <person displayName="bruno merven" id="{91699B87-187B-4A09-BB94-559E01E0E64C}" userId="144eb91ed0ec6402" providerId="Windows Live"/>
 </personList>
 </file>
@@ -4782,6 +4799,9 @@
   <threadedComment ref="C13" dT="2020-03-26T13:06:59.96" personId="{91699B87-187B-4A09-BB94-559E01E0E64C}" id="{6BC8B301-C25D-4243-8984-1D8083FBD633}">
     <text>from Bryce, linked to amount of coke used for combustion.</text>
   </threadedComment>
+  <threadedComment ref="E14" dT="2021-05-27T19:21:07.86" personId="{B37ECF2F-7DD9-4573-B8C3-8678149F6950}" id="{F057E6D1-F0A4-43AE-A671-8DD980C81287}">
+    <text>adjusted to Match FBC coefficient - see TCH_PWR</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -4800,10 +4820,10 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5275,11 +5295,11 @@
       <c r="C14" s="1">
         <v>96.25</v>
       </c>
-      <c r="D14" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1.4E-3</v>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="F14" s="1">
         <v>0.62619999999999998</v>
@@ -5298,7 +5318,7 @@
       </c>
       <c r="K14">
         <f>SUMPRODUCT($C$1:$J$1,C14:J14)</f>
-        <v>96.704999999999998</v>
+        <v>122.91</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -7051,8 +7071,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C1:AF480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13111,15 +13131,15 @@
       </c>
       <c r="E112">
         <f>IF($P112&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J112,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F112">
         <f>IF($P112&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J112,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1.4E-3</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="G112">
         <f>IF(P112&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J112,Factors!$B$5:$B$61,0)),0))</f>
-        <v>96.704999999999998</v>
+        <v>122.91</v>
       </c>
       <c r="J112" t="str">
         <f t="shared" si="9"/>

</xml_diff>

<commit_message>
More Fixes done, mainly in CCS. Linked Model running to 2050.
</commit_message>
<xml_diff>
--- a/EmissionFactors.xlsx
+++ b/EmissionFactors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305078AD-40A9-4026-92C4-ED6A500AAB8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F356A46-5E89-42FF-8EA2-223A6C9E0748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="195" windowWidth="25230" windowHeight="14940" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
+    <workbookView xWindow="1500" yWindow="-17055" windowWidth="25605" windowHeight="14325" activeTab="1" xr2:uid="{F7D82C8E-DCA0-4D7B-A715-D4A1F93CE55E}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -7071,8 +7071,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C1:AF480"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
+      <selection activeCell="D369" sqref="D369:G369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25895,21 +25895,17 @@
       <c r="C367" t="s">
         <v>724</v>
       </c>
-      <c r="D367">
-        <f>IF($P367&gt;0,0,IFERROR(INDEX(Factors!$C$5:$C$61,MATCH($J367,Factors!$B$5:$B$61,0)),0))</f>
-        <v>56.1</v>
-      </c>
-      <c r="E367">
-        <f>IF($P367&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J367,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1E-3</v>
-      </c>
-      <c r="F367">
-        <f>IF($P367&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J367,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1E-4</v>
-      </c>
-      <c r="G367">
-        <f>IF(P367&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J367,Factors!$B$5:$B$61,0)),0))</f>
-        <v>56.152000000000001</v>
+      <c r="D367" s="8">
+        <v>0</v>
+      </c>
+      <c r="E367" s="8">
+        <v>0</v>
+      </c>
+      <c r="F367" s="8">
+        <v>0</v>
+      </c>
+      <c r="G367" s="8">
+        <v>0</v>
       </c>
       <c r="J367" t="str">
         <f t="shared" si="41"/>
@@ -25991,21 +25987,17 @@
       <c r="C369" t="s">
         <v>728</v>
       </c>
-      <c r="D369">
-        <f>IF($P369&gt;0,0,IFERROR(INDEX(Factors!$C$5:$C$61,MATCH($J369,Factors!$B$5:$B$61,0)),0))</f>
-        <v>63.1</v>
-      </c>
-      <c r="E369">
-        <f>IF($P369&gt;0,0,IFERROR(INDEX(Factors!$D$5:$D$61,MATCH($J369,Factors!$B$5:$B$61,0)),0))</f>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F369">
-        <f>IF($P369&gt;0,0,IFERROR(INDEX(Factors!$E$5:$E$61,MATCH($J369,Factors!$B$5:$B$61,0)),0))</f>
-        <v>1E-4</v>
-      </c>
-      <c r="G369">
-        <f>IF(P369&gt;0,0,IFERROR(INDEX(Factors!$K$5:$K$61,MATCH(J369,Factors!$B$5:$B$61,0)),0))</f>
-        <v>63.194000000000003</v>
+      <c r="D369" s="8">
+        <v>0</v>
+      </c>
+      <c r="E369" s="8">
+        <v>0</v>
+      </c>
+      <c r="F369" s="8">
+        <v>0</v>
+      </c>
+      <c r="G369" s="8">
+        <v>0</v>
       </c>
       <c r="J369" t="str">
         <f t="shared" si="41"/>

</xml_diff>